<commit_message>
a lot of advance in final PCB
</commit_message>
<xml_diff>
--- a/Platine/Neue_Pumpe/Test_PCB/Platte/Artikelliste.xlsx
+++ b/Platine/Neue_Pumpe/Test_PCB/Platte/Artikelliste.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huawei\Documents\GitHub\ConVacuumSystem\Platine\Platte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huawei\Documents\GitHub\ConVacuumSystem\Platine\Neue_Pumpe\Test_PCB\Platte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E083C46D-4B38-41B2-8413-DC1D6B824152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCDE28C-075A-464E-9148-C454E3B04ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Artikelnummer</t>
   </si>
@@ -172,12 +172,6 @@
   </si>
   <si>
     <t>B/N</t>
-  </si>
-  <si>
-    <t>790-EADOGM204SA</t>
-  </si>
-  <si>
-    <t>LCD-Zeichenanzeigemodule und Zubehör 4x20 - 4.83mm, black&amp;white negative</t>
   </si>
   <si>
     <t>Stck</t>
@@ -227,6 +221,24 @@
   <si>
     <t>Fass</t>
   </si>
+  <si>
+    <t>200-FLE10501GDVKTR</t>
+  </si>
+  <si>
+    <t>Platine-zu-Platine &amp; Mezzanine-Steckverbinder Cost Effective Surface Mount Socket, 0.050" Pitch</t>
+  </si>
+  <si>
+    <t>200-FTSH10501LDVK</t>
+  </si>
+  <si>
+    <t>Sockel &amp; Kabelgehäuse High Reliability Header Strips, .050" pitch</t>
+  </si>
+  <si>
+    <t>667-ERA-3AEB2800V</t>
+  </si>
+  <si>
+    <t>Dünnfilmwiderstände - SMD 0603 280ohm 0.1% 25ppm</t>
+  </si>
 </sst>
 </file>
 
@@ -235,7 +247,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,11 +293,6 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -612,7 +619,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -657,7 +664,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -877,7 +883,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -915,44 +921,69 @@
     </row>
     <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="8">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="8">
-        <v>6</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" s="10">
-        <v>27.59</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F2" s="11"/>
       <c r="G2" s="12"/>
       <c r="H2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="39"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="40"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="40">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="40">
+        <v>2.36</v>
+      </c>
       <c r="F3" s="11"/>
       <c r="G3" s="41"/>
-      <c r="H3" s="42"/>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17"/>
+      <c r="A4" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="15">
+        <v>20</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="17">
+        <v>7.4999999999999997E-2</v>
+      </c>
       <c r="F4" s="18"/>
       <c r="G4" s="19"/>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="13"/>
@@ -2729,7 +2760,7 @@
           <x14:formula1>
             <xm:f>Tabelle2!$A$1:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>D2 D4:D100</xm:sqref>
+          <xm:sqref>D2 D5:D100</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2750,77 +2781,77 @@
   <sheetData>
     <row r="1" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="37" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="37" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="37" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="37" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="37" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="37" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="37" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="37" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="37" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="37" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="37" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="37" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="37" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="37" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="37" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>